<commit_message>
yêu cầu an toàn
</commit_message>
<xml_diff>
--- a/Phân tích/Yêu cầu nghiệp vụ.xlsx
+++ b/Phân tích/Yêu cầu nghiệp vụ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auhai\Documents\GitHub\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D4F85A-4F34-4F59-9EF1-DF8EB6D3B122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07E190F-1ED5-43A0-8265-E57C585285B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{CA4F4A45-B080-403D-880F-8A1956738ABC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA4F4A45-B080-403D-880F-8A1956738ABC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="148">
   <si>
     <t>STT</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>- Danh mục nhân viên</t>
-  </si>
-  <si>
-    <t>-Danh mục  đơn đặt hàng</t>
   </si>
   <si>
     <t>- Danh mục  khách hàng</t>
@@ -870,7 +867,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="A1:D37"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +890,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="I1" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -917,16 +914,16 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -949,10 +946,10 @@
         <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="M3" s="5"/>
     </row>
@@ -976,10 +973,10 @@
         <v>2</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="M4" s="5"/>
     </row>
@@ -1003,10 +1000,10 @@
         <v>3</v>
       </c>
       <c r="K5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="M5" s="5"/>
     </row>
@@ -1030,10 +1027,10 @@
         <v>4</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M6" s="5"/>
     </row>
@@ -1058,7 +1055,7 @@
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M7" s="5"/>
     </row>
@@ -1083,7 +1080,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M8" s="5"/>
     </row>
@@ -1092,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -1104,11 +1101,11 @@
         <v>7</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M9" s="5"/>
     </row>
@@ -1117,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -1129,11 +1126,11 @@
         <v>8</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M10" s="5"/>
     </row>
@@ -1142,7 +1139,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1154,11 +1151,11 @@
         <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M11" s="5"/>
     </row>
@@ -1167,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1179,11 +1176,11 @@
         <v>10</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M12" s="5"/>
     </row>
@@ -1192,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>34</v>
@@ -1204,11 +1201,11 @@
         <v>11</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M13" s="5"/>
     </row>
@@ -1217,7 +1214,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
@@ -1229,13 +1226,13 @@
         <v>12</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M14" s="5"/>
     </row>
@@ -1244,7 +1241,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -1256,13 +1253,13 @@
         <v>13</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M15" s="5"/>
     </row>
@@ -1271,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>37</v>
@@ -1283,13 +1280,13 @@
         <v>14</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M16" s="5"/>
     </row>
@@ -1298,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>38</v>
@@ -1310,13 +1307,13 @@
         <v>15</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M17" s="5"/>
     </row>
@@ -1325,7 +1322,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>39</v>
@@ -1337,13 +1334,13 @@
         <v>16</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M18" s="5"/>
     </row>
@@ -1352,7 +1349,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>40</v>
@@ -1364,13 +1361,13 @@
         <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M19" s="5"/>
     </row>
@@ -1379,7 +1376,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>41</v>
@@ -1391,13 +1388,13 @@
         <v>18</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="M20" s="5"/>
     </row>
@@ -1406,7 +1403,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>42</v>
@@ -1418,13 +1415,13 @@
         <v>19</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M21" s="5"/>
     </row>
@@ -1448,10 +1445,10 @@
         <v>6</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M22" s="5"/>
     </row>
@@ -1476,7 +1473,7 @@
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M23" s="5"/>
     </row>
@@ -1500,10 +1497,10 @@
         <v>8</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M24" s="5"/>
     </row>
@@ -1527,10 +1524,10 @@
         <v>9</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M25" s="5"/>
     </row>
@@ -1555,7 +1552,7 @@
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M26" s="5"/>
     </row>
@@ -1579,10 +1576,10 @@
         <v>11</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M27" s="5"/>
     </row>
@@ -1607,7 +1604,7 @@
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M28" s="5"/>
     </row>
@@ -1631,10 +1628,10 @@
         <v>13</v>
       </c>
       <c r="K29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L29" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="M29" s="5"/>
     </row>
@@ -1659,7 +1656,7 @@
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M30" s="5"/>
     </row>
@@ -1683,10 +1680,10 @@
         <v>15</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M31" s="5"/>
     </row>
@@ -1710,10 +1707,10 @@
         <v>16</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M32" s="5"/>
     </row>
@@ -1737,10 +1734,10 @@
         <v>17</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M33" s="5"/>
     </row>
@@ -1764,10 +1761,10 @@
         <v>18</v>
       </c>
       <c r="K34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="M34" s="5"/>
     </row>
@@ -1791,10 +1788,10 @@
         <v>19</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M35" s="5"/>
     </row>
@@ -1803,25 +1800,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I36" s="1">
         <v>35</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M36" s="5"/>
     </row>
@@ -1830,25 +1827,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I37" s="1">
         <v>36</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M37" s="5"/>
     </row>

</xml_diff>

<commit_message>
làm giao diện QLDM - Tài khoản, thêm BM35,QD935, Thêm trong yêu cầu nghiệp vụ
</commit_message>
<xml_diff>
--- a/Phân tích/Yêu cầu nghiệp vụ.xlsx
+++ b/Phân tích/Yêu cầu nghiệp vụ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Phân tích\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CNPM\Phân tích\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB4DEF9-AB9A-4232-8687-CC4B6E8850E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D7E12-5F6D-4F7C-9BCB-3711F75330D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{CA4F4A45-B080-403D-880F-8A1956738ABC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CA4F4A45-B080-403D-880F-8A1956738ABC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="148">
   <si>
     <t>STT</t>
   </si>
@@ -454,6 +454,21 @@
   </si>
   <si>
     <t>QĐ33</t>
+  </si>
+  <si>
+    <t>Danh mục tài khoản</t>
+  </si>
+  <si>
+    <t>BM35</t>
+  </si>
+  <si>
+    <t>QD35</t>
+  </si>
+  <si>
+    <t>Cung cấp tài khoản cho nhân viên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xuất danh mục tài khoản và lưu </t>
   </si>
 </sst>
 </file>
@@ -848,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8C8E8B-6B0E-4DFD-82F0-66B3E2D3D432}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,6 +1820,30 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I37" s="1">
+        <v>35</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="M37" s="4"/>
     </row>
   </sheetData>

</xml_diff>